<commit_message>
Modificacion sobre concentrado de metricas Mayo
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-150529.xlsx
+++ b/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-150529.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\proyecto\qualtcom\Organizacional\Medicion y Monitoreo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Organizacional\Medicion y Monitoreo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835"/>
+    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Desviacion de esfuerzo" sheetId="6" r:id="rId1"/>
@@ -227,7 +227,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,6 +267,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,7 +458,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -481,9 +493,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -540,17 +549,32 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -653,98 +677,7 @@
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
     <cellStyle name="Porcentaje 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="90">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="77">
     <dxf>
       <fill>
         <patternFill>
@@ -1398,10 +1331,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>140</c:v>
+                  <c:v>91.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>45.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>45.600000000000009</c:v>
@@ -1526,11 +1459,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="325232096"/>
-        <c:axId val="325231536"/>
+        <c:axId val="288273584"/>
+        <c:axId val="288275824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="325232096"/>
+        <c:axId val="288273584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1540,7 +1473,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="325231536"/>
+        <c:crossAx val="288275824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1548,7 +1481,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="325231536"/>
+        <c:axId val="288275824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1492,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="325232096"/>
+        <c:crossAx val="288273584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1675,11 +1608,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="278474784"/>
-        <c:axId val="278473664"/>
+        <c:axId val="397921856"/>
+        <c:axId val="397922416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="278474784"/>
+        <c:axId val="397921856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1689,7 +1622,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="278473664"/>
+        <c:crossAx val="397922416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1697,7 +1630,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="278473664"/>
+        <c:axId val="397922416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1709,7 +1642,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="278474784"/>
+        <c:crossAx val="397921856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1970,11 +1903,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="432948272"/>
-        <c:axId val="432945472"/>
+        <c:axId val="295795072"/>
+        <c:axId val="295795632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="432948272"/>
+        <c:axId val="295795072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1984,7 +1917,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="432945472"/>
+        <c:crossAx val="295795632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1992,7 +1925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="432945472"/>
+        <c:axId val="295795632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2004,7 +1937,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="432948272"/>
+        <c:crossAx val="295795072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2138,10 +2071,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.7857142857142857</c:v>
+                  <c:v>0.67105263157894735</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.97142857142857142</c:v>
+                  <c:v>0.91228070175438591</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.82456140350877194</c:v>
@@ -2176,11 +2109,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="4426192"/>
-        <c:axId val="4422832"/>
+        <c:axId val="402450784"/>
+        <c:axId val="153036720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="4426192"/>
+        <c:axId val="402450784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2190,7 +2123,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4422832"/>
+        <c:crossAx val="153036720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2198,7 +2131,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4422832"/>
+        <c:axId val="153036720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2211,7 +2144,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4426192"/>
+        <c:crossAx val="402450784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2304,7 +2237,7 @@
                 <c:formatCode>_-"$"* #,##0.00_-;\-"$"* #,##0.00_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11653</c:v>
+                  <c:v>9989</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5693.7300000000005</c:v>
@@ -2354,7 +2287,7 @@
                 <c:formatCode>_-"$"* #,##0.00_-;\-"$"* #,##0.00_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3666.56</c:v>
+                  <c:v>1415.08</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>861.16600000000005</c:v>
@@ -2377,11 +2310,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="4423392"/>
-        <c:axId val="4421712"/>
+        <c:axId val="290009744"/>
+        <c:axId val="290010304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="4423392"/>
+        <c:axId val="290009744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2391,7 +2324,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4421712"/>
+        <c:crossAx val="290010304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2399,7 +2332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4421712"/>
+        <c:axId val="290010304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2410,7 +2343,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4423392"/>
+        <c:crossAx val="290009744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2508,7 +2441,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.68535484424611692</c:v>
+                  <c:v>0.85833616978676541</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.84875187267397645</c:v>
@@ -2531,11 +2464,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="4426752"/>
-        <c:axId val="4425632"/>
+        <c:axId val="103784800"/>
+        <c:axId val="103785360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="4426752"/>
+        <c:axId val="103784800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2545,7 +2478,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4425632"/>
+        <c:crossAx val="103785360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2553,7 +2486,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4425632"/>
+        <c:axId val="103785360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2566,7 +2499,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4426752"/>
+        <c:crossAx val="103784800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2677,11 +2610,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="325426112"/>
-        <c:axId val="325429472"/>
+        <c:axId val="297380448"/>
+        <c:axId val="297381008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="325426112"/>
+        <c:axId val="297380448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2691,7 +2624,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="325429472"/>
+        <c:crossAx val="297381008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2699,7 +2632,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="325429472"/>
+        <c:axId val="297381008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2710,7 +2643,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="325426112"/>
+        <c:crossAx val="297380448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2827,11 +2760,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="325428912"/>
-        <c:axId val="325427232"/>
+        <c:axId val="297383808"/>
+        <c:axId val="295349584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="325428912"/>
+        <c:axId val="297383808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2841,7 +2774,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="325427232"/>
+        <c:crossAx val="295349584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2849,7 +2782,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="325427232"/>
+        <c:axId val="295349584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2861,7 +2794,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="325428912"/>
+        <c:crossAx val="297383808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2984,11 +2917,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="431604448"/>
-        <c:axId val="431603888"/>
+        <c:axId val="295352384"/>
+        <c:axId val="295352944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="431604448"/>
+        <c:axId val="295352384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2998,7 +2931,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431603888"/>
+        <c:crossAx val="295352944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3006,7 +2939,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="431603888"/>
+        <c:axId val="295352944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3018,7 +2951,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431604448"/>
+        <c:crossAx val="295352384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3135,11 +3068,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="431605568"/>
-        <c:axId val="431605008"/>
+        <c:axId val="369826192"/>
+        <c:axId val="369826752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="431605568"/>
+        <c:axId val="369826192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3149,7 +3082,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431605008"/>
+        <c:crossAx val="369826752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3157,7 +3090,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="431605008"/>
+        <c:axId val="369826752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3169,7 +3102,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="431605568"/>
+        <c:crossAx val="369826192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3286,11 +3219,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="278471984"/>
-        <c:axId val="278471424"/>
+        <c:axId val="103862432"/>
+        <c:axId val="103862992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="278471984"/>
+        <c:axId val="103862432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3300,7 +3233,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="278471424"/>
+        <c:crossAx val="103862992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3308,7 +3241,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="278471424"/>
+        <c:axId val="103862992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3320,7 +3253,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="278471984"/>
+        <c:crossAx val="103862432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3363,7 +3296,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3399,7 +3332,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3442,7 +3375,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3480,7 +3413,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3523,7 +3456,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3559,7 +3492,7 @@
         <xdr:cNvPr id="7" name="6 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3600,7 +3533,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3636,7 +3569,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3677,7 +3610,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3720,7 +3653,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4067,8 +4000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4104,131 +4037,131 @@
     <row r="17" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:22" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="16" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="38">
-        <v>140</v>
-      </c>
-      <c r="E20" s="38">
+      <c r="D20" s="37">
+        <v>91.2</v>
+      </c>
+      <c r="E20" s="37">
         <v>30</v>
       </c>
-      <c r="F20" s="39">
+      <c r="F20" s="42">
         <f>(D20-E20)/D20</f>
-        <v>0.7857142857142857</v>
+        <v>0.67105263157894735</v>
       </c>
     </row>
     <row r="21" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="43"/>
-      <c r="C21" s="17" t="s">
+      <c r="B21" s="40"/>
+      <c r="C21" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="38">
-        <v>140</v>
-      </c>
-      <c r="E21" s="38">
+      <c r="D21" s="37">
+        <v>45.6</v>
+      </c>
+      <c r="E21" s="37">
         <v>4</v>
       </c>
-      <c r="F21" s="39">
+      <c r="F21" s="42">
         <f t="shared" ref="F21:F26" si="0">(D21-E21)/D21</f>
-        <v>0.97142857142857142</v>
+        <v>0.91228070175438591</v>
       </c>
     </row>
     <row r="22" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="38">
+      <c r="D22" s="37">
         <v>45.600000000000009</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="37">
         <v>8</v>
       </c>
-      <c r="F22" s="39">
+      <c r="F22" s="42">
         <f t="shared" si="0"/>
         <v>0.82456140350877194</v>
       </c>
     </row>
     <row r="23" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="43"/>
-      <c r="C23" s="17" t="s">
+      <c r="B23" s="40"/>
+      <c r="C23" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="37">
         <v>91.200000000000017</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="37">
         <v>11.3</v>
       </c>
-      <c r="F23" s="39">
+      <c r="F23" s="42">
         <f t="shared" si="0"/>
         <v>0.87609649122807021</v>
       </c>
     </row>
     <row r="24" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="37">
+      <c r="C24" s="35"/>
+      <c r="D24" s="36">
         <v>1</v>
       </c>
-      <c r="E24" s="37">
+      <c r="E24" s="36">
         <v>1</v>
       </c>
-      <c r="F24" s="41">
+      <c r="F24" s="43">
         <f>(D24-E24)/D24</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="37">
+      <c r="C25" s="35"/>
+      <c r="D25" s="36">
         <v>2</v>
       </c>
-      <c r="E25" s="37">
+      <c r="E25" s="36">
         <v>1.6</v>
       </c>
-      <c r="F25" s="41">
+      <c r="F25" s="43">
         <f t="shared" si="0"/>
         <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="26" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="37">
+      <c r="C26" s="35"/>
+      <c r="D26" s="36">
         <v>0.5</v>
       </c>
-      <c r="E26" s="42">
+      <c r="E26" s="39">
         <v>0.17</v>
       </c>
-      <c r="F26" s="41">
+      <c r="F26" s="44">
         <f t="shared" si="0"/>
         <v>0.65999999999999992</v>
       </c>
@@ -4717,7 +4650,7 @@
     <mergeCell ref="B20:B21"/>
   </mergeCells>
   <conditionalFormatting sqref="A29:XFD1048576">
-    <cfRule type="cellIs" dxfId="78" priority="63" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="76" priority="63" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison5!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4737,7 +4670,7 @@
   <dimension ref="B1:E31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E21" sqref="E20:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4791,14 +4724,14 @@
         <v>3</v>
       </c>
       <c r="C20" s="15">
-        <v>11653</v>
+        <v>9989</v>
       </c>
       <c r="D20" s="15">
-        <v>3666.56</v>
-      </c>
-      <c r="E20" s="16">
+        <v>1415.08</v>
+      </c>
+      <c r="E20" s="41">
         <f>(C20-D20)/C20</f>
-        <v>0.68535484424611692</v>
+        <v>0.85833616978676541</v>
       </c>
     </row>
     <row r="21" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -4811,7 +4744,7 @@
       <c r="D21" s="15">
         <v>861.16600000000005</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="41">
         <f t="shared" ref="E21" si="0">(C21-D21)/C21</f>
         <v>0.84875187267397645</v>
       </c>
@@ -4828,7 +4761,7 @@
     <row r="31" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A27:XFD1048576">
-    <cfRule type="cellIs" dxfId="77" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="75" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison5!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4844,7 +4777,7 @@
   <dimension ref="B2:P25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H4" sqref="H4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4864,107 +4797,107 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>150228</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>150331</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>150430</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="17">
         <v>150529</v>
       </c>
-      <c r="H3" s="25"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="18">
+      <c r="B4" s="17">
         <v>1</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="22">
         <v>1</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <v>1</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="22">
         <v>1</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="22">
         <v>1</v>
       </c>
-      <c r="H4" s="26">
+      <c r="H4" s="45">
         <f>AVERAGE(D4:G4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="18">
+      <c r="B5" s="17">
         <v>2</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <v>0.8</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="22">
         <v>1</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="22">
         <v>1</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="45">
         <f>AVERAGE(D5:G5)</f>
         <v>0.93333333333333324</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="18">
+      <c r="B6" s="17">
         <v>3</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="26" t="e">
+      <c r="G6" s="22"/>
+      <c r="H6" s="25" t="e">
         <f>AVERAGE(D6:F6)</f>
         <v>#DIV/0!</v>
       </c>
@@ -4974,100 +4907,100 @@
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="21" t="s">
         <v>7</v>
       </c>
       <c r="P8" s="5"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="30">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="29">
         <v>150227</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <v>150331</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
         <v>150330</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="17">
         <v>150529</v>
       </c>
-      <c r="H9" s="27"/>
+      <c r="H9" s="26"/>
       <c r="P9" s="5"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="18">
+      <c r="B10" s="17">
         <v>1</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="28" t="e">
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="27" t="e">
         <f t="shared" ref="H10:H12" si="0">AVERAGE(D10:F10)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="18">
+      <c r="B11" s="17">
         <v>2</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="28" t="e">
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="27" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="18">
+      <c r="B12" s="17">
         <v>3</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="28" t="e">
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="27" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -5075,87 +5008,87 @@
     <row r="25" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A3:C3 N2:XFD6 A9:A12 A15:XFD1048576 A8:B8 A4:H6 A2:E2 A7:I7 I8 A13:I14 K7:XFD14 H9:I12 H2">
-    <cfRule type="cellIs" dxfId="76" priority="24" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="74" priority="24" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="75" priority="20" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="73" priority="20" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="74" priority="19" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="72" priority="19" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="73" priority="11" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="71" priority="11" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="72" priority="17" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="70" priority="17" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:G12">
-    <cfRule type="cellIs" dxfId="71" priority="15" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="69" priority="15" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C12">
-    <cfRule type="cellIs" dxfId="70" priority="14" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="68" priority="14" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="69" priority="12" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="67" priority="12" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="68" priority="10" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="66" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="67" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="65" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="66" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="64" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="65" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="63" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="64" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="62" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G2">
-    <cfRule type="cellIs" dxfId="63" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="61" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G3">
-    <cfRule type="cellIs" dxfId="62" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="60" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="59" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="58" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5175,7 +5108,7 @@
   <dimension ref="B2:J40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H4" sqref="H4:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5193,65 +5126,65 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>150228</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>150331</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>150430</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="17">
         <v>150529</v>
       </c>
-      <c r="H3" s="25"/>
+      <c r="H3" s="24"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>1</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>1</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>1</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="23">
         <v>1</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="46">
         <f>AVERAGE(D4:G4)</f>
         <v>1</v>
       </c>
@@ -5259,25 +5192,25 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>2</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>1</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <v>1</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>1</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="23">
         <v>1</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="46">
         <f>AVERAGE(D5:G5)</f>
         <v>1</v>
       </c>
@@ -5285,25 +5218,25 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <v>3</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="23">
         <v>1</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="23">
         <v>1</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="23">
         <v>1</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="23">
         <v>1</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="46">
         <f>AVERAGE(D6:G6)</f>
         <v>1</v>
       </c>
@@ -5311,25 +5244,25 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="20">
+      <c r="B7" s="19">
         <v>4</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="23">
         <v>1</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="23">
         <v>1</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="23">
         <v>1</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="46">
         <f>AVERAGE(D7:G7)</f>
         <v>1</v>
       </c>
@@ -5337,75 +5270,75 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="30" t="s">
         <v>7</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="30">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="29">
         <v>150227</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="17">
         <v>150331</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <v>150430</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="17">
         <v>150529</v>
       </c>
-      <c r="H10" s="27"/>
+      <c r="H10" s="26"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="20">
+      <c r="B11" s="19">
         <v>1</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="26" t="e">
+      <c r="G11" s="22"/>
+      <c r="H11" s="25" t="e">
         <f t="shared" ref="H11:H13" si="0">AVERAGE(D11:F11)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5413,23 +5346,23 @@
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="20">
+      <c r="B12" s="19">
         <v>2</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="26" t="e">
+      <c r="G12" s="22"/>
+      <c r="H12" s="25" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -5437,23 +5370,23 @@
       <c r="J12" s="9"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="20">
+      <c r="B13" s="19">
         <v>3</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="26" t="e">
+      <c r="G13" s="22"/>
+      <c r="H13" s="25" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -5495,127 +5428,127 @@
     <sortCondition descending="1" ref="C29"/>
   </sortState>
   <conditionalFormatting sqref="K2:XFD11 A2:A12 I2:J3 I12:XFD12 A14:XFD15 A19:XFD1048576 A16:B18 D16:XFD18">
-    <cfRule type="cellIs" dxfId="61" priority="34" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="57" priority="34" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 B9 B2:D2 H10:H13 C4:H6 H2">
-    <cfRule type="cellIs" dxfId="60" priority="33" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="56" priority="33" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="59" priority="30" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="55" priority="30" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="58" priority="31" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="54" priority="31" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="57" priority="24" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="53" priority="24" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:D13">
-    <cfRule type="cellIs" dxfId="56" priority="28" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="52" priority="28" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="55" priority="27" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="51" priority="27" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C13">
-    <cfRule type="cellIs" dxfId="54" priority="23" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="50" priority="23" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6">
-    <cfRule type="cellIs" dxfId="53" priority="22" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="49" priority="22" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B13">
-    <cfRule type="cellIs" dxfId="52" priority="21" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="48" priority="21" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:G13">
-    <cfRule type="cellIs" dxfId="51" priority="18" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="47" priority="18" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="50" priority="17" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="46" priority="17" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="49" priority="15" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="45" priority="15" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="48" priority="14" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="44" priority="14" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="47" priority="12" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="43" priority="12" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="46" priority="10" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="42" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="45" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="41" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:H8">
-    <cfRule type="cellIs" dxfId="44" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="40" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B8">
-    <cfRule type="cellIs" dxfId="43" priority="7" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="39" priority="7" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="42" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="38" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="41" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="37" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G2">
-    <cfRule type="cellIs" dxfId="40" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="36" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G3">
-    <cfRule type="cellIs" dxfId="39" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="35" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="38" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="34" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="cellIs" dxfId="37" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="33" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5634,7 +5567,7 @@
   <dimension ref="B2:J34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G6"/>
+      <selection activeCell="H4" sqref="H4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5652,65 +5585,65 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="28" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>150227</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>150331</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>150430</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="17">
         <v>150529</v>
       </c>
-      <c r="H3" s="25"/>
+      <c r="H3" s="24"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>1</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>1</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>1</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="23">
         <v>1</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="46">
         <f>AVERAGE(D4:G4)</f>
         <v>1</v>
       </c>
@@ -5718,25 +5651,25 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>2</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>1</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <v>1</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>1</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="23">
         <v>1</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="46">
         <f>AVERAGE(D5:G5)</f>
         <v>1</v>
       </c>
@@ -5744,25 +5677,25 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <v>3</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="28" t="e">
+      <c r="H6" s="27" t="e">
         <f>AVERAGE(D6:G6)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5808,57 +5741,57 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A7 I2:J3 A8:XFD9 A13:XFD1048576 A10:B12 D10:XFD12 J7:XFD7 K2:XFD6">
-    <cfRule type="cellIs" dxfId="36" priority="24" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="32" priority="24" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 B2:D2 B7:G7 H2 C4:E6 G4:H6">
-    <cfRule type="cellIs" dxfId="35" priority="23" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="31" priority="23" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6">
-    <cfRule type="cellIs" dxfId="34" priority="15" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="30" priority="15" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="33" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="29" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="32" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="28" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="31" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="27" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="cellIs" dxfId="30" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="29" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="25" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F6">
-    <cfRule type="cellIs" dxfId="28" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="24" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="27" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="23" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="26" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="22" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5872,7 +5805,7 @@
   <dimension ref="B2:J34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H4" sqref="H4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5890,65 +5823,65 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="28" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>150227</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>150331</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>150430</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="17">
         <v>150529</v>
       </c>
-      <c r="H3" s="25"/>
+      <c r="H3" s="24"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>0.75</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>1</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>1</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="23">
         <v>1</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="46">
         <f>AVERAGE(D4:G4)</f>
         <v>0.9375</v>
       </c>
@@ -5956,25 +5889,25 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>2</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>1</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <v>1</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>1</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="23">
         <v>1</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="46">
         <f>AVERAGE(D5:G5)</f>
         <v>1</v>
       </c>
@@ -5982,25 +5915,25 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <v>3</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="28" t="e">
+      <c r="H6" s="27" t="e">
         <f>AVERAGE(D6:G6)</f>
         <v>#DIV/0!</v>
       </c>
@@ -6046,57 +5979,57 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A7 I2:J3 A8:XFD9 A13:XFD1048576 A10:B12 D10:XFD12 J7:XFD7 K2:XFD6">
-    <cfRule type="cellIs" dxfId="25" priority="14" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="21" priority="14" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 B2:D2 B7:G7 H2 C4:E6 G4:H6">
-    <cfRule type="cellIs" dxfId="24" priority="13" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="20" priority="13" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6">
-    <cfRule type="cellIs" dxfId="23" priority="12" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="19" priority="12" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="22" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="18" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="21" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="20" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="16" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="cellIs" dxfId="19" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="18" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="14" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F6">
-    <cfRule type="cellIs" dxfId="17" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="13" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="16" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="15" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6109,8 +6042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6121,168 +6054,168 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="28" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="30">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="29">
         <v>150227</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>150331</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="29">
         <v>150430</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="29">
         <v>150529</v>
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <v>1</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="47">
         <v>0.88</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="47">
         <v>0.94</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>2</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="47">
         <v>0.91</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="47">
         <v>0.97</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <v>3</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="47">
         <v>1</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="47">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="20">
+      <c r="C7" s="19">
         <v>4</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="47">
         <v>0.88</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="47">
         <v>0.94</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3 C2:E2 D4:G6 G2">
-    <cfRule type="cellIs" dxfId="14" priority="12" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="12" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C6">
-    <cfRule type="cellIs" dxfId="13" priority="11" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="11" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="12" priority="10" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="11" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="10" priority="7" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="9" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:G7">
-    <cfRule type="cellIs" dxfId="8" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H6 H2">
-    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="5" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Concentrado de metricas Mayo, actualizado por errores de escritura encontrados internamente
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-150529.xlsx
+++ b/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-150529.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Organizacional\Medicion y Monitoreo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\Documents\qtp\qualtcom\Organizacional\Medicion y Monitoreo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835"/>
   </bookViews>
   <sheets>
     <sheet name="Desviacion de esfuerzo" sheetId="6" r:id="rId1"/>
@@ -555,9 +555,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -575,6 +572,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="8" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1459,11 +1459,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="288273584"/>
-        <c:axId val="288275824"/>
+        <c:axId val="321199200"/>
+        <c:axId val="321199760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="288273584"/>
+        <c:axId val="321199200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1473,7 +1473,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288275824"/>
+        <c:crossAx val="321199760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1481,7 +1481,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288275824"/>
+        <c:axId val="321199760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1492,7 +1492,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288273584"/>
+        <c:crossAx val="321199200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1544,7 +1544,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1608,11 +1607,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="397921856"/>
-        <c:axId val="397922416"/>
+        <c:axId val="321616320"/>
+        <c:axId val="321616880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="397921856"/>
+        <c:axId val="321616320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1622,7 +1621,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="397922416"/>
+        <c:crossAx val="321616880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1630,7 +1629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397922416"/>
+        <c:axId val="321616880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1642,7 +1641,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="397921856"/>
+        <c:crossAx val="321616320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1903,11 +1902,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="295795072"/>
-        <c:axId val="295795632"/>
+        <c:axId val="411153344"/>
+        <c:axId val="411153904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="295795072"/>
+        <c:axId val="411153344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1917,7 +1916,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="295795632"/>
+        <c:crossAx val="411153904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1925,7 +1924,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="295795632"/>
+        <c:axId val="411153904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1937,7 +1936,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="295795072"/>
+        <c:crossAx val="411153344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2109,11 +2108,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="402450784"/>
-        <c:axId val="153036720"/>
+        <c:axId val="321202560"/>
+        <c:axId val="321203120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="402450784"/>
+        <c:axId val="321202560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2123,7 +2122,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153036720"/>
+        <c:crossAx val="321203120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2131,7 +2130,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153036720"/>
+        <c:axId val="321203120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2144,7 +2143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="402450784"/>
+        <c:crossAx val="321202560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2310,11 +2309,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="290009744"/>
-        <c:axId val="290010304"/>
+        <c:axId val="321205920"/>
+        <c:axId val="321206480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="290009744"/>
+        <c:axId val="321205920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2324,7 +2323,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="290010304"/>
+        <c:crossAx val="321206480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2332,7 +2331,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="290010304"/>
+        <c:axId val="321206480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2343,7 +2342,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="290009744"/>
+        <c:crossAx val="321205920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2464,11 +2463,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="103784800"/>
-        <c:axId val="103785360"/>
+        <c:axId val="321209280"/>
+        <c:axId val="321209840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103784800"/>
+        <c:axId val="321209280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2478,7 +2477,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103785360"/>
+        <c:crossAx val="321209840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2486,7 +2485,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103785360"/>
+        <c:axId val="321209840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2499,7 +2498,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103784800"/>
+        <c:crossAx val="321209280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2610,11 +2609,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="297380448"/>
-        <c:axId val="297381008"/>
+        <c:axId val="321212080"/>
+        <c:axId val="321212640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="297380448"/>
+        <c:axId val="321212080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2624,7 +2623,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297381008"/>
+        <c:crossAx val="321212640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2632,7 +2631,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297381008"/>
+        <c:axId val="321212640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2643,7 +2642,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297380448"/>
+        <c:crossAx val="321212080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2760,11 +2759,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="297383808"/>
-        <c:axId val="295349584"/>
+        <c:axId val="321602880"/>
+        <c:axId val="321603440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="297383808"/>
+        <c:axId val="321602880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2774,7 +2773,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="295349584"/>
+        <c:crossAx val="321603440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2782,7 +2781,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="295349584"/>
+        <c:axId val="321603440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2794,7 +2793,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297383808"/>
+        <c:crossAx val="321602880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2847,7 +2846,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2917,11 +2915,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="295352384"/>
-        <c:axId val="295352944"/>
+        <c:axId val="321606240"/>
+        <c:axId val="321606800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="295352384"/>
+        <c:axId val="321606240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2931,7 +2929,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="295352944"/>
+        <c:crossAx val="321606800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2939,7 +2937,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="295352944"/>
+        <c:axId val="321606800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2951,7 +2949,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="295352384"/>
+        <c:crossAx val="321606240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3004,7 +3002,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3068,11 +3065,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="369826192"/>
-        <c:axId val="369826752"/>
+        <c:axId val="321609600"/>
+        <c:axId val="321610160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="369826192"/>
+        <c:axId val="321609600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3082,7 +3079,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="369826752"/>
+        <c:crossAx val="321610160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3090,7 +3087,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="369826752"/>
+        <c:axId val="321610160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3102,7 +3099,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="369826192"/>
+        <c:crossAx val="321609600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3155,7 +3152,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3219,11 +3215,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="103862432"/>
-        <c:axId val="103862992"/>
+        <c:axId val="321612960"/>
+        <c:axId val="321613520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103862432"/>
+        <c:axId val="321612960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3233,7 +3229,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103862992"/>
+        <c:crossAx val="321613520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3241,7 +3237,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103862992"/>
+        <c:axId val="321613520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3253,7 +3249,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103862432"/>
+        <c:crossAx val="321612960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3296,7 +3292,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3332,7 +3328,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3375,7 +3371,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3413,7 +3409,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3456,7 +3452,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3492,7 +3488,7 @@
         <xdr:cNvPr id="7" name="6 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3533,7 +3529,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3569,7 +3565,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3610,7 +3606,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3653,7 +3649,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4000,8 +3996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4038,7 +4034,7 @@
     <row r="18" spans="2:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:22" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>0</v>
@@ -4051,7 +4047,7 @@
       </c>
     </row>
     <row r="20" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="47" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="16" t="s">
@@ -4063,13 +4059,13 @@
       <c r="E20" s="37">
         <v>30</v>
       </c>
-      <c r="F20" s="42">
+      <c r="F20" s="41">
         <f>(D20-E20)/D20</f>
         <v>0.67105263157894735</v>
       </c>
     </row>
     <row r="21" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="16" t="s">
         <v>5</v>
       </c>
@@ -4079,13 +4075,13 @@
       <c r="E21" s="37">
         <v>4</v>
       </c>
-      <c r="F21" s="42">
+      <c r="F21" s="41">
         <f t="shared" ref="F21:F26" si="0">(D21-E21)/D21</f>
         <v>0.91228070175438591</v>
       </c>
     </row>
     <row r="22" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="47" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="16" t="s">
@@ -4097,13 +4093,13 @@
       <c r="E22" s="37">
         <v>8</v>
       </c>
-      <c r="F22" s="42">
+      <c r="F22" s="41">
         <f t="shared" si="0"/>
         <v>0.82456140350877194</v>
       </c>
     </row>
     <row r="23" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="40"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="16" t="s">
         <v>5</v>
       </c>
@@ -4113,7 +4109,7 @@
       <c r="E23" s="37">
         <v>11.3</v>
       </c>
-      <c r="F23" s="42">
+      <c r="F23" s="41">
         <f t="shared" si="0"/>
         <v>0.87609649122807021</v>
       </c>
@@ -4129,7 +4125,7 @@
       <c r="E24" s="36">
         <v>1</v>
       </c>
-      <c r="F24" s="43">
+      <c r="F24" s="42">
         <f>(D24-E24)/D24</f>
         <v>0</v>
       </c>
@@ -4145,7 +4141,7 @@
       <c r="E25" s="36">
         <v>1.6</v>
       </c>
-      <c r="F25" s="43">
+      <c r="F25" s="42">
         <f t="shared" si="0"/>
         <v>0.19999999999999996</v>
       </c>
@@ -4161,7 +4157,7 @@
       <c r="E26" s="39">
         <v>0.17</v>
       </c>
-      <c r="F26" s="44">
+      <c r="F26" s="43">
         <f t="shared" si="0"/>
         <v>0.65999999999999992</v>
       </c>
@@ -4670,7 +4666,7 @@
   <dimension ref="B1:E31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E21" sqref="E20:E21"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4707,7 +4703,7 @@
     <row r="18" spans="2:5" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:5" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>0</v>
@@ -4729,7 +4725,7 @@
       <c r="D20" s="15">
         <v>1415.08</v>
       </c>
-      <c r="E20" s="41">
+      <c r="E20" s="40">
         <f>(C20-D20)/C20</f>
         <v>0.85833616978676541</v>
       </c>
@@ -4744,7 +4740,7 @@
       <c r="D21" s="15">
         <v>861.16600000000005</v>
       </c>
-      <c r="E21" s="41">
+      <c r="E21" s="40">
         <f t="shared" ref="E21" si="0">(C21-D21)/C21</f>
         <v>0.84875187267397645</v>
       </c>
@@ -4851,7 +4847,7 @@
       <c r="G4" s="22">
         <v>1</v>
       </c>
-      <c r="H4" s="45">
+      <c r="H4" s="44">
         <f>AVERAGE(D4:G4)</f>
         <v>1</v>
       </c>
@@ -4875,7 +4871,7 @@
       <c r="G5" s="22">
         <v>1</v>
       </c>
-      <c r="H5" s="45">
+      <c r="H5" s="44">
         <f>AVERAGE(D5:G5)</f>
         <v>0.93333333333333324</v>
       </c>
@@ -5184,7 +5180,7 @@
       <c r="G4" s="23">
         <v>1</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <f>AVERAGE(D4:G4)</f>
         <v>1</v>
       </c>
@@ -5210,7 +5206,7 @@
       <c r="G5" s="23">
         <v>1</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="45">
         <f>AVERAGE(D5:G5)</f>
         <v>1</v>
       </c>
@@ -5236,7 +5232,7 @@
       <c r="G6" s="23">
         <v>1</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="45">
         <f>AVERAGE(D6:G6)</f>
         <v>1</v>
       </c>
@@ -5262,7 +5258,7 @@
       <c r="G7" s="23">
         <v>1</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="45">
         <f>AVERAGE(D7:G7)</f>
         <v>1</v>
       </c>
@@ -5643,7 +5639,7 @@
       <c r="G4" s="23">
         <v>1</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <f>AVERAGE(D4:G4)</f>
         <v>1</v>
       </c>
@@ -5669,7 +5665,7 @@
       <c r="G5" s="23">
         <v>1</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="45">
         <f>AVERAGE(D5:G5)</f>
         <v>1</v>
       </c>
@@ -5881,7 +5877,7 @@
       <c r="G4" s="23">
         <v>1</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <f>AVERAGE(D4:G4)</f>
         <v>0.9375</v>
       </c>
@@ -5907,7 +5903,7 @@
       <c r="G5" s="23">
         <v>1</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="45">
         <f>AVERAGE(D5:G5)</f>
         <v>1</v>
       </c>
@@ -6042,7 +6038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8:J8"/>
     </sheetView>
   </sheetViews>
@@ -6096,10 +6092,10 @@
       <c r="F4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="46">
         <v>0.88</v>
       </c>
-      <c r="H4" s="47">
+      <c r="H4" s="46">
         <v>0.94</v>
       </c>
     </row>
@@ -6116,10 +6112,10 @@
       <c r="F5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="47">
+      <c r="G5" s="46">
         <v>0.91</v>
       </c>
-      <c r="H5" s="47">
+      <c r="H5" s="46">
         <v>0.97</v>
       </c>
     </row>
@@ -6136,10 +6132,10 @@
       <c r="F6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="47">
+      <c r="G6" s="46">
         <v>1</v>
       </c>
-      <c r="H6" s="47">
+      <c r="H6" s="46">
         <v>1</v>
       </c>
     </row>
@@ -6156,10 +6152,10 @@
       <c r="F7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="47">
+      <c r="G7" s="46">
         <v>0.88</v>
       </c>
-      <c r="H7" s="47">
+      <c r="H7" s="46">
         <v>0.94</v>
       </c>
     </row>

</xml_diff>